<commit_message>
[ADDITIVE] Updated the final report with content to chapters 3 and 4.
</commit_message>
<xml_diff>
--- a/Administrative/Final Report Statistics.xlsx
+++ b/Administrative/Final Report Statistics.xlsx
@@ -725,6 +725,25 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Task</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1159,7 +1178,7 @@
   <dimension ref="A3:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[PERFECTIVE] Updated the statistics and the final report slides with new figures.
</commit_message>
<xml_diff>
--- a/Administrative/Final Report Statistics.xlsx
+++ b/Administrative/Final Report Statistics.xlsx
@@ -337,10 +337,10 @@
                   <c:v>62.85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.05</c:v>
+                  <c:v>93.55</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,11 +355,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108472960"/>
-        <c:axId val="108479232"/>
+        <c:axId val="106441344"/>
+        <c:axId val="106447616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108472960"/>
+        <c:axId val="106441344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,7 +387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108479232"/>
+        <c:crossAx val="106447616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -395,7 +395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108479232"/>
+        <c:axId val="106447616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,7 +425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108472960"/>
+        <c:crossAx val="106441344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -573,16 +573,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>85.3</c:v>
+                  <c:v>96.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.25</c:v>
+                  <c:v>88.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>37.75</c:v>
@@ -715,11 +715,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108513920"/>
-        <c:axId val="108519808"/>
+        <c:axId val="106494592"/>
+        <c:axId val="106562304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108513920"/>
+        <c:axId val="106494592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,7 +747,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108519808"/>
+        <c:crossAx val="106562304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -755,7 +755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108519808"/>
+        <c:axId val="106562304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +785,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108513920"/>
+        <c:crossAx val="106494592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1178,7 +1178,7 @@
   <dimension ref="A3:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,7 +1257,7 @@
         <v>192</v>
       </c>
       <c r="M4">
-        <v>85.3</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1277,10 +1277,10 @@
         <v>62.85</v>
       </c>
       <c r="F5">
-        <v>93.05</v>
+        <v>93.55</v>
       </c>
       <c r="G5">
-        <v>35</v>
+        <v>55.5</v>
       </c>
       <c r="J5" t="s">
         <v>12</v>
@@ -1292,7 +1292,7 @@
         <v>80</v>
       </c>
       <c r="M5">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1320,7 +1320,7 @@
         <v>170</v>
       </c>
       <c r="M7">
-        <v>84.25</v>
+        <v>88.25</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[ADDITIVE] Added the status report from May. Updated the final report with time usage figures.
</commit_message>
<xml_diff>
--- a/Administrative/Final Report Statistics.xlsx
+++ b/Administrative/Final Report Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Planned</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Apr 2013</t>
+  </si>
+  <si>
+    <t>May 2013</t>
   </si>
 </sst>
 </file>
@@ -175,33 +178,14 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Monthly Planned vs. Realized Time Usage</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -225,9 +209,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$G$3</c:f>
+              <c:f>Sheet1!$B$3:$H$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Nov 2012</c:v>
                 </c:pt>
@@ -245,16 +229,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Apr 2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>May 2013</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$G$4</c:f>
+              <c:f>Sheet1!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>66</c:v>
                 </c:pt>
@@ -272,6 +259,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -294,9 +284,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$G$3</c:f>
+              <c:f>Sheet1!$B$3:$H$3</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Nov 2012</c:v>
                 </c:pt>
@@ -314,16 +304,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Apr 2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>May 2013</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$G$5</c:f>
+              <c:f>Sheet1!$B$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>26.35</c:v>
                 </c:pt>
@@ -341,6 +334,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,11 +351,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="106441344"/>
-        <c:axId val="106447616"/>
+        <c:axId val="107960576"/>
+        <c:axId val="107962752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106441344"/>
+        <c:axId val="107960576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,7 +383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106447616"/>
+        <c:crossAx val="107962752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -395,7 +391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106447616"/>
+        <c:axId val="107962752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -405,7 +401,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:bodyPr rot="0" vert="wordArtVert"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -425,7 +421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106441344"/>
+        <c:crossAx val="107960576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -454,34 +450,14 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Working Hour Distribution</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -573,7 +549,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>96.3</c:v>
+                  <c:v>104.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>41</c:v>
@@ -715,11 +691,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="106494592"/>
-        <c:axId val="106562304"/>
+        <c:axId val="109381888"/>
+        <c:axId val="109400448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106494592"/>
+        <c:axId val="109381888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,7 +704,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:bodyPr rot="0" vert="wordArtVert"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -747,7 +723,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106562304"/>
+        <c:crossAx val="109400448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -755,7 +731,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106562304"/>
+        <c:axId val="109400448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +761,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106494592"/>
+        <c:crossAx val="109381888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -812,13 +788,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>295273</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
+      <xdr:colOff>1428749</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -841,16 +817,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>419099</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1178,15 +1154,15 @@
   <dimension ref="A3:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="37.5703125" customWidth="1"/>
     <col min="10" max="10" width="5.5703125" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" customWidth="1"/>
@@ -1212,6 +1188,9 @@
       <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1247,6 +1226,9 @@
       <c r="G4">
         <v>60</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
@@ -1257,7 +1239,7 @@
         <v>192</v>
       </c>
       <c r="M4">
-        <v>96.3</v>
+        <v>104.55</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1281,6 +1263,9 @@
       </c>
       <c r="G5">
         <v>55.5</v>
+      </c>
+      <c r="H5">
+        <v>6.5</v>
       </c>
       <c r="J5" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
[PERFECTIVE] Updated all documents.
</commit_message>
<xml_diff>
--- a/Administrative/Final Report Statistics.xlsx
+++ b/Administrative/Final Report Statistics.xlsx
@@ -336,7 +336,7 @@
                   <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,11 +351,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="107960576"/>
-        <c:axId val="107962752"/>
+        <c:axId val="106314368"/>
+        <c:axId val="106324736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107960576"/>
+        <c:axId val="106314368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -383,7 +383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107962752"/>
+        <c:crossAx val="106324736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -391,7 +391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107962752"/>
+        <c:axId val="106324736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,7 +421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107960576"/>
+        <c:crossAx val="106314368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -435,6 +435,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -549,10 +559,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>104.55</c:v>
+                  <c:v>111.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19</c:v>
@@ -691,11 +701,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="109381888"/>
-        <c:axId val="109400448"/>
+        <c:axId val="106371328"/>
+        <c:axId val="106385792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109381888"/>
+        <c:axId val="106371328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +733,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109400448"/>
+        <c:crossAx val="106385792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -731,7 +741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109400448"/>
+        <c:axId val="106385792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +771,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109381888"/>
+        <c:crossAx val="106371328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -775,6 +785,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -788,15 +808,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>295273</xdr:colOff>
+      <xdr:colOff>295272</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1428749</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>214311</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>107841</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -817,16 +837,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>109537</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>20792</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1153,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W60" sqref="W59:W60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,7 +1259,7 @@
         <v>192</v>
       </c>
       <c r="M4">
-        <v>104.55</v>
+        <v>111.05</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1265,7 +1285,7 @@
         <v>55.5</v>
       </c>
       <c r="H5">
-        <v>6.5</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
         <v>12</v>
@@ -1277,7 +1297,7 @@
         <v>80</v>
       </c>
       <c r="M5">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>